<commit_message>
check num cols and rows in tests - clean column with 20% missing values
</commit_message>
<xml_diff>
--- a/server/tests/files_to_test/students_list_excel/example_excel_hebrew_7_students.xlsx
+++ b/server/tests/files_to_test/students_list_excel/example_excel_hebrew_7_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar_Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\server\tests\files_to_test\students_list_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F40DB64-9F96-4123-9FF8-8968C2BD4850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A82F56-47C9-4948-84EA-FBF40020ED00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="D1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +498,7 @@
     <row r="6" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G6" s="1"/>
       <c r="H6">
-        <v>530342423</v>
+        <v>530342425</v>
       </c>
       <c r="I6" s="1">
         <v>305696031</v>

</xml_diff>